<commit_message>
Updated the Chrome driver
</commit_message>
<xml_diff>
--- a/reports/ExcelReport/ExtentExcel.xlsx
+++ b/reports/ExcelReport/ExtentExcel.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
   <si>
     <t>Duration</t>
   </si>
@@ -277,19 +277,22 @@
     <t>device</t>
   </si>
   <si>
-    <t>Nov 26, 2024 2:19:03 pm</t>
+    <t>Feb 10, 2025 2:53:49 PM</t>
   </si>
   <si>
-    <t>Nov 26, 2024 2:17:52 pm</t>
+    <t>Feb 10, 2025 2:52:08 PM</t>
   </si>
   <si>
-    <t>Nov 26, 2024 2:18:54 pm</t>
+    <t>Feb 10, 2025 2:53:46 PM</t>
   </si>
   <si>
-    <t>1 m 2.011 s</t>
+    <t>1 m 37.714 s</t>
   </si>
   <si>
     <t>0%</t>
+  </si>
+  <si>
+    <t>10%</t>
   </si>
   <si>
     <t>Validate e-commerce mobile application functionality</t>
@@ -298,47 +301,21 @@
     <t>Search for a product on the e-commerce website</t>
   </si>
   <si>
-    <t>59.591 s</t>
+    <t>1 m 37.032 s</t>
   </si>
   <si>
-    <t>59.629 s</t>
+    <t>1 m 37.040 s</t>
   </si>
   <si>
-    <t>StepDefinition.Hooks.setup()</t>
+    <t>When the user clicks the respective searched product it should navigated to product details page</t>
   </si>
   <si>
-    <t xml:space="preserve">org.openqa.selenium.SessionNotCreatedException: Could not start a new session. Response code 500. Message: An unknown server-side error occurred while processing the command. Original error: A new session could not be created. Details: session not created: This version of ChromeDriver only supports Chrome version 131
-Current browser version is 124.0.6367.219 with package name com.android.chrome 
-Host info: host: 'DESKTOP-JEHOL2V', ip: '192.168.2.224'
-Build info: version: '4.26.0', revision: '8ccf0219d7'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.2'
-Driver info: io.appium.java_client.android.AndroidDriver
-Command: [null, newSession {capabilities=[Capabilities {appium:automationName: UiAutomator2, appium:chromedriverExecutable: C:\Users\Balaji\IdeaProject..., appium:connectHardwareKeyboard: true, appium:deviceName: AutomationEmulator, appium:ensureWebviewsHavePages: true, appium:nativeWebScreenshot: true, appium:newCommandTimeout: 3600, appium:platformVersion: 15, browserName: Chrome, platformName: ANDROID}]}]
-Capabilities {appium:automationName: UiAutomator2, appium:chromedriverExecutable: C:\Users\Balaji\IdeaProject..., appium:connectHardwareKeyboard: true, appium:deviceName: AutomationEmulator, appium:ensureWebviewsHavePages: true, appium:nativeWebScreenshot: true, appium:newCommandTimeout: 3600, appium:platformVersion: 15, browserName: Chrome, platformName: ANDROID}
-	at org.openqa.selenium.remote.ProtocolHandshake.createSession(ProtocolHandshake.java:114)
-	at org.openqa.selenium.remote.ProtocolHandshake.createSession(ProtocolHandshake.java:75)
-	at org.openqa.selenium.remote.ProtocolHandshake.createSession(ProtocolHandshake.java:61)
-	at io.appium.java_client.remote.AppiumCommandExecutor.createSession(AppiumCommandExecutor.java:176)
-	at io.appium.java_client.remote.AppiumCommandExecutor.execute(AppiumCommandExecutor.java:237)
-	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:545)
-	at io.appium.java_client.AppiumDriver.startSession(AppiumDriver.java:270)
-	at org.openqa.selenium.remote.RemoteWebDriver.&lt;init&gt;(RemoteWebDriver.java:174)
-	at io.appium.java_client.AppiumDriver.&lt;init&gt;(AppiumDriver.java:91)
-	at io.appium.java_client.AppiumDriver.&lt;init&gt;(AppiumDriver.java:103)
-	at io.appium.java_client.android.AndroidDriver.&lt;init&gt;(AndroidDriver.java:109)
-	at ProjectBase.TestBaseClass.launchAndroidApp(TestBaseClass.java:66)
-	at ProjectBase.TestBaseClass.SuiteBeforeMethods(TestBaseClass.java:45)
-	at StepDefinition.Hooks.setup(Hooks.java:22)
-</t>
-  </si>
-  <si>
-    <t>StepDefinition.Hooks.teardown()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">java.lang.IllegalStateException: Driver has not been initialized. Call setDriver() first.
-	at ProjectBase.TestBaseClass.getDriver(TestBaseClass.java:232)
-	at ProjectBase.TestBaseClass.teardown(TestBaseClass.java:270)
-	at StepDefinition.Hooks.teardown(Hooks.java:28)
+    <t xml:space="preserve">java.lang.AssertionError: Unable to click the element using js click method
+	at org.testng.Assert.fail(Assert.java:111)
+	at ProjectBase.TestBaseClass.jsClick(TestBaseClass.java:180)
+	at PageObjects.SearchResultPage.Click_Product_Displayed_On_Search_Result_Page(SearchResultPage.java:65)
+	at StepDefinition.Hana_T1049_Web_Checkout_Page_Functionality.the_user_clicks_the_respective_searched_product_it_should_navigated_to_product_details_page(Hana_T1049_Web_Checkout_Page_Functionality.java:72)
+	at ✽.the user clicks the respective searched product it should navigated to product details page(file:///C:/Users/sakrateesh/Desktop/Hana_POS_Mobile_Automation/src/test/resources/Features/Bestflorist.feature:17)
 </t>
   </si>
 </sst>
@@ -2363,7 +2340,12 @@
           <c:val>
             <c:numRef>
               <c:f>'DB Data'!$R$20</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2434,7 +2416,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>70.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2504,7 +2486,12 @@
           <c:val>
             <c:numRef>
               <c:f>'DB Data'!$S$20</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -3479,7 +3466,12 @@
           <c:val>
             <c:numRef>
               <c:f>Scenarios!$H$22</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -3549,7 +3541,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>70.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3628,7 +3620,12 @@
           <c:val>
             <c:numRef>
               <c:f>Scenarios!$I$22</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -8218,14 +8215,14 @@
     </row>
     <row r="39">
       <c r="B39" s="71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="69"/>
       <c r="D39" s="72" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F39" s="69"/>
       <c r="G39" s="72" t="s">
@@ -8233,7 +8230,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="9E55" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="E72F" scenarios="true" objects="true"/>
   <mergeCells count="4">
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E38:F38"/>
@@ -8314,16 +8311,16 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="73" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="74" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" s="73" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F22" s="72" t="s">
         <v>41</v>
@@ -8331,10 +8328,14 @@
       <c r="G22" s="70" t="n">
         <v>70.0</v>
       </c>
-      <c r="H22" s="75"/>
-      <c r="I22" s="76"/>
+      <c r="H22" s="75" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I22" s="76" t="n">
+        <v>1.0</v>
+      </c>
       <c r="J22" s="77" t="n">
-        <v>70.0</v>
+        <v>62.0</v>
       </c>
     </row>
   </sheetData>
@@ -8431,13 +8432,13 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="73" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E22" s="70" t="n">
         <v>1.0</v>
@@ -8453,10 +8454,14 @@
       <c r="J22" s="70" t="n">
         <v>70.0</v>
       </c>
-      <c r="K22" s="75"/>
-      <c r="L22" s="76"/>
+      <c r="K22" s="75" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="L22" s="76" t="n">
+        <v>1.0</v>
+      </c>
       <c r="M22" s="77" t="n">
-        <v>70.0</v>
+        <v>62.0</v>
       </c>
     </row>
   </sheetData>
@@ -8473,7 +8478,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="2.0" state="frozen" topLeftCell="A3" activePane="bottomLeft"/>
@@ -8504,34 +8509,20 @@
     </row>
     <row r="3">
       <c r="B3" s="71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="71" t="s">
         <v>79</v>
-      </c>
-      <c r="E4" s="71" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="F003" scenarios="true" objects="true"/>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-  </mergeCells>
+  <sheetProtection sheet="true" password="8029" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8594,7 +8585,9 @@
       <c r="G2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="H2" s="0"/>
+      <c r="H2" t="n" s="0">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
@@ -8618,7 +8611,9 @@
       <c r="G3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="H3" s="0"/>
+      <c r="H3" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
@@ -8639,7 +8634,7 @@
         <v>14</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>70.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -8685,7 +8680,7 @@
         <v>72</v>
       </c>
       <c r="H6" s="39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -8757,7 +8752,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="69" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I20" s="69" t="s">
         <v>41</v>
@@ -8768,15 +8763,19 @@
       </c>
       <c r="L20" s="70"/>
       <c r="P20" s="69" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q20" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="R20" s="70"/>
-      <c r="S20" s="70"/>
+      <c r="R20" s="70" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="S20" s="70" t="n">
+        <v>1.0</v>
+      </c>
       <c r="T20" s="70" t="n">
-        <v>70.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>